<commit_message>
Auto commit 30-05-2025 13:26:06.96
</commit_message>
<xml_diff>
--- a/GWD Data/Hydrants.xlsx
+++ b/GWD Data/Hydrants.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="49">
   <si>
     <t>Hydrants with tap  (for common use of size 0.8 x 0.5 m platform)</t>
   </si>
@@ -246,79 +246,85 @@
 </t>
   </si>
   <si>
+    <t>day</t>
+  </si>
+  <si>
+    <t>/day</t>
+  </si>
+  <si>
+    <t>Beldar (0114)</t>
+  </si>
+  <si>
+    <t>Sub Total</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total  for labour </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total   </t>
+  </si>
+  <si>
+    <t>Hydrants with tap  ( for individual families of size 0.6 X 0.3 M platform)</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Merriweather"/>
+        <color theme="1"/>
+        <sz val="12.0"/>
+      </rPr>
+      <t>110 mm 4kg/cm</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Merriweather"/>
+        <color theme="1"/>
+        <sz val="12.0"/>
+        <vertAlign val="superscript"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Merriweather"/>
+        <color theme="1"/>
+        <sz val="12.0"/>
+      </rPr>
+      <t xml:space="preserve"> PVC Pipe (MR55)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Merriweather"/>
+        <color theme="1"/>
+        <sz val="12.0"/>
+      </rPr>
+      <t>32mm 10kg/cm</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Merriweather"/>
+        <color theme="1"/>
+        <sz val="12.0"/>
+        <vertAlign val="superscript"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Merriweather"/>
+        <color theme="1"/>
+        <sz val="12.0"/>
+      </rPr>
+      <t xml:space="preserve"> PVC Pipe (MR44)</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve"> PVC tap (MR10048)</t>
+  </si>
+  <si>
     <t>Nos</t>
-  </si>
-  <si>
-    <t>Beldar (0114)</t>
-  </si>
-  <si>
-    <t>Sub Total</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Total  for labour </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Total   </t>
-  </si>
-  <si>
-    <t>Hydrants with tap  ( for individual families of size 0.6 X 0.3 M platform)</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Merriweather"/>
-        <color theme="1"/>
-        <sz val="12.0"/>
-      </rPr>
-      <t>110 mm 4kg/cm</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Merriweather"/>
-        <color theme="1"/>
-        <sz val="12.0"/>
-        <vertAlign val="superscript"/>
-      </rPr>
-      <t>2</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Merriweather"/>
-        <color theme="1"/>
-        <sz val="12.0"/>
-      </rPr>
-      <t xml:space="preserve"> PVC Pipe (MR55)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Merriweather"/>
-        <color theme="1"/>
-        <sz val="12.0"/>
-      </rPr>
-      <t>32mm 10kg/cm</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Merriweather"/>
-        <color theme="1"/>
-        <sz val="12.0"/>
-        <vertAlign val="superscript"/>
-      </rPr>
-      <t>2</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Merriweather"/>
-        <color theme="1"/>
-        <sz val="12.0"/>
-      </rPr>
-      <t xml:space="preserve"> PVC Pipe (MR44)</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve"> PVC tap (MR10048)</t>
   </si>
   <si>
     <r>
@@ -1240,14 +1246,14 @@
       <c r="C18" s="4">
         <v>0.22</v>
       </c>
-      <c r="D18" s="4" t="s">
+      <c r="D18" s="8" t="s">
         <v>29</v>
       </c>
       <c r="E18" s="8">
         <v>784.0</v>
       </c>
-      <c r="F18" s="4" t="s">
-        <v>7</v>
+      <c r="F18" s="8" t="s">
+        <v>30</v>
       </c>
       <c r="G18" s="6">
         <f t="shared" si="3"/>
@@ -1257,19 +1263,19 @@
     <row r="19">
       <c r="A19" s="12"/>
       <c r="B19" s="7" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C19" s="4">
         <v>0.22</v>
       </c>
-      <c r="D19" s="4" t="s">
+      <c r="D19" s="8" t="s">
         <v>29</v>
       </c>
       <c r="E19" s="8">
         <v>645.0</v>
       </c>
-      <c r="F19" s="4" t="s">
-        <v>7</v>
+      <c r="F19" s="8" t="s">
+        <v>30</v>
       </c>
       <c r="G19" s="6">
         <f t="shared" si="3"/>
@@ -1279,7 +1285,7 @@
     <row r="20">
       <c r="A20" s="4"/>
       <c r="B20" s="5" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C20" s="4"/>
       <c r="D20" s="4"/>
@@ -1335,7 +1341,7 @@
     <row r="24">
       <c r="A24" s="4"/>
       <c r="B24" s="4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C24" s="4"/>
       <c r="D24" s="4"/>
@@ -1349,7 +1355,7 @@
     <row r="25">
       <c r="A25" s="4"/>
       <c r="B25" s="13" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C25" s="4"/>
       <c r="D25" s="4"/>
@@ -1374,7 +1380,7 @@
     </row>
     <row r="27">
       <c r="A27" s="14" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
@@ -1388,7 +1394,7 @@
         <v>1.0</v>
       </c>
       <c r="B28" s="16" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C28" s="15">
         <v>110.0</v>
@@ -1412,7 +1418,7 @@
         <v>2.0</v>
       </c>
       <c r="B29" s="16" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C29" s="15">
         <v>150.0</v>
@@ -1436,7 +1442,7 @@
         <v>3.0</v>
       </c>
       <c r="B30" s="18" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C30" s="15">
         <v>1.0</v>
@@ -1490,7 +1496,7 @@
         <v>2.0</v>
       </c>
       <c r="D32" s="15" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="E32" s="15">
         <v>45.0</v>
@@ -1508,7 +1514,7 @@
         <v>6.0</v>
       </c>
       <c r="B33" s="16" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C33" s="15">
         <v>1.0</v>
@@ -1624,13 +1630,13 @@
         <v>8.0</v>
       </c>
       <c r="B40" s="16" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C40" s="15">
         <v>0.054</v>
       </c>
       <c r="D40" s="15" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="E40" s="19">
         <v>249.03</v>
@@ -1654,7 +1660,7 @@
         <v>0.08</v>
       </c>
       <c r="D41" s="15" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="E41" s="21">
         <v>6393.89</v>
@@ -1678,13 +1684,13 @@
         <v>0.18</v>
       </c>
       <c r="D42" s="15" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="E42" s="19">
         <v>267.33</v>
       </c>
       <c r="F42" s="15" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="G42" s="17">
         <f t="shared" si="6"/>
@@ -1702,13 +1708,13 @@
         <v>0.36</v>
       </c>
       <c r="D43" s="15" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="E43" s="19">
         <v>255.98</v>
       </c>
       <c r="F43" s="15" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="G43" s="22">
         <f t="shared" si="6"/>
@@ -1726,7 +1732,7 @@
         <v>0.22</v>
       </c>
       <c r="D44" s="15" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="E44" s="19">
         <v>784.0</v>
@@ -1742,13 +1748,13 @@
     <row r="45">
       <c r="A45" s="12"/>
       <c r="B45" s="18" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C45" s="15">
         <v>0.22</v>
       </c>
       <c r="D45" s="15" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="E45" s="19">
         <v>645.0</v>
@@ -1764,7 +1770,7 @@
     <row r="46">
       <c r="A46" s="15"/>
       <c r="B46" s="16" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C46" s="15"/>
       <c r="D46" s="15"/>
@@ -1820,7 +1826,7 @@
     <row r="50">
       <c r="A50" s="15"/>
       <c r="B50" s="15" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C50" s="15"/>
       <c r="D50" s="15"/>
@@ -1834,7 +1840,7 @@
     <row r="51">
       <c r="A51" s="15"/>
       <c r="B51" s="24" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C51" s="15"/>
       <c r="D51" s="15"/>

</xml_diff>